<commit_message>
tiered seeding edits and edward's proof explanation
</commit_message>
<xml_diff>
--- a/thesis-tex/references.xlsx
+++ b/thesis-tex/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D965A0-A0E4-4877-936D-F4A31B70F5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5982D9-512F-4056-8B74-A005E685B7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{708375FB-6962-4B20-A84D-3D0BF229F98B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>Title</t>
   </si>
@@ -250,6 +250,18 @@
   </si>
   <si>
     <t>reseeding is ordered</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://www-jstor-org.ezp-prod1.hul.harvard.edu/stable/pdf/2286606.pdf?refreqid=excelsior%3Ac6f9f27cd7701f5e7471bf45a00f7c81&amp;ab_segments=&amp;origin=&amp;initiator=&amp;acceptTC=1</t>
+  </si>
+  <si>
+    <t>Do Stronger Players Win More Knockout Tournaments</t>
+  </si>
+  <si>
+    <t>defined ordered</t>
   </si>
 </sst>
 </file>
@@ -610,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C99330B-41D4-434B-87B1-F3F6E5AC9A2D}">
-  <dimension ref="B4:H19"/>
+  <dimension ref="B4:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,9 +675,6 @@
       <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
       <c r="H5" t="s">
         <v>22</v>
       </c>
@@ -812,6 +821,9 @@
       <c r="C12" t="s">
         <v>47</v>
       </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
       <c r="E12" t="s">
         <v>45</v>
       </c>
@@ -963,6 +975,29 @@
       </c>
       <c r="H19" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>1978</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -971,5 +1006,6 @@
     <sortCondition ref="F5:F19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Developing reseeding and messing around with /G and /W
</commit_message>
<xml_diff>
--- a/thesis-tex/references.xlsx
+++ b/thesis-tex/references.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3D3292-8A57-43EE-A0A0-5C28A3692E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638CE450-0B6F-4506-A289-BE13AE43BC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{708375FB-6962-4B20-A84D-3D0BF229F98B}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -639,7 +640,7 @@
   <dimension ref="B4:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,7 +823,7 @@
         <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Fleshing out efficient multibrackets to include prize structures
</commit_message>
<xml_diff>
--- a/thesis-tex/references.xlsx
+++ b/thesis-tex/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DC60B5-28D1-458C-8E36-10A00ACA60E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1509886C-6787-478C-9D2E-36C00F10294B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{708375FB-6962-4B20-A84D-3D0BF229F98B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
   <si>
     <t>Title</t>
   </si>
@@ -291,6 +291,21 @@
   </si>
   <si>
     <t>proving 8-balanced is not ordered</t>
+  </si>
+  <si>
+    <t>https://ajc.maths.uq.edu.au/pdf/20/ocr-ajc-v20-p19.pdf</t>
+  </si>
+  <si>
+    <t>Landau's Theorem revisited</t>
+  </si>
+  <si>
+    <t>Jerrold Griggs, K. B. Reid</t>
+  </si>
+  <si>
+    <t>Round Robins</t>
+  </si>
+  <si>
+    <t>nice proof</t>
   </si>
 </sst>
 </file>
@@ -651,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C99330B-41D4-434B-87B1-F3F6E5AC9A2D}">
-  <dimension ref="B4:H22"/>
+  <dimension ref="B4:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,6 +1090,29 @@
         <v>79</v>
       </c>
     </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23">
+        <v>1999</v>
+      </c>
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:H22">
     <sortCondition descending="1" ref="G5:G22"/>

</xml_diff>

<commit_message>
network formats first half
</commit_message>
<xml_diff>
--- a/thesis-tex/references.xlsx
+++ b/thesis-tex/references.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFBC121-0A7C-4068-9A4D-282F99984362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FFAF6E-A412-4E95-82B5-D0C8C5F74CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{708375FB-6962-4B20-A84D-3D0BF229F98B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>Title</t>
   </si>
@@ -306,6 +306,15 @@
   </si>
   <si>
     <t>nice proof</t>
+  </si>
+  <si>
+    <t>Dabney things</t>
+  </si>
+  <si>
+    <t>Lewis Carol</t>
+  </si>
+  <si>
+    <t>Art of computing</t>
   </si>
 </sst>
 </file>
@@ -666,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C99330B-41D4-434B-87B1-F3F6E5AC9A2D}">
-  <dimension ref="B4:H23"/>
+  <dimension ref="B4:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,6 +1122,21 @@
         <v>89</v>
       </c>
     </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:H22">
     <sortCondition descending="1" ref="G5:G22"/>

</xml_diff>

<commit_message>
Update to third-place games
</commit_message>
<xml_diff>
--- a/thesis-tex/references.xlsx
+++ b/thesis-tex/references.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FFAF6E-A412-4E95-82B5-D0C8C5F74CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16FC4FB-337E-4F06-A08A-496B892F8146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{708375FB-6962-4B20-A84D-3D0BF229F98B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="99">
   <si>
     <t>Title</t>
   </si>
@@ -314,7 +314,25 @@
     <t>Lewis Carol</t>
   </si>
   <si>
-    <t>Art of computing</t>
+    <t>The Art of Computer Programing</t>
+  </si>
+  <si>
+    <t>Donald Knuth</t>
+  </si>
+  <si>
+    <t>https://doc.lagout.org/science/0_Computer%20Science/2_Algorithms/The%20Art%20of%20Computer%20Programming%20%28vol.%203_%20Sorting%20and%20Searching%29%20%282nd%20ed.%29%20%5BKnuth%201998-05-04%5D.pdf</t>
+  </si>
+  <si>
+    <t>Multibrackets</t>
+  </si>
+  <si>
+    <t>networked</t>
+  </si>
+  <si>
+    <t>https://www-degruyter-com.ezp-prod1.hul.harvard.edu/document/doi/10.1515/jqas-2012-0055/pdf?stream=true</t>
+  </si>
+  <si>
+    <t>(double elim designs?)</t>
   </si>
 </sst>
 </file>
@@ -675,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C99330B-41D4-434B-87B1-F3F6E5AC9A2D}">
-  <dimension ref="B4:H28"/>
+  <dimension ref="B4:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,19 +1140,45 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24">
+        <v>1938</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>92</v>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>